<commit_message>
added the upload_to_google_drive method, and main() file to run everything
</commit_message>
<xml_diff>
--- a/technicalFactorsExcel/sp500topDownFactors.xlsx
+++ b/technicalFactorsExcel/sp500topDownFactors.xlsx
@@ -508,22 +508,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.2169354838709678</v>
+        <v>1.362096774193548</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.432258064516129</v>
+        <v>1.530645161290322</v>
       </c>
       <c r="E2" t="n">
-        <v>-3.430645161290323</v>
+        <v>-2.050806451612903</v>
       </c>
       <c r="F2" t="n">
-        <v>7.316129032258064</v>
+        <v>9.741935483870968</v>
       </c>
       <c r="G2" t="n">
-        <v>-3.574193548387097</v>
+        <v>-2.245161290322581</v>
       </c>
       <c r="H2" t="n">
-        <v>-4.437096774193547</v>
+        <v>-3.092741935483871</v>
       </c>
     </row>
     <row r="3">
@@ -534,22 +534,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.09112903225806457</v>
+        <v>0.4548387096774194</v>
       </c>
       <c r="D3" t="n">
-        <v>1.29758064516129</v>
+        <v>2.263709677419354</v>
       </c>
       <c r="E3" t="n">
-        <v>4.445161290322581</v>
+        <v>4.882258064516127</v>
       </c>
       <c r="F3" t="n">
-        <v>19.37741935483871</v>
+        <v>19.81209677419354</v>
       </c>
       <c r="G3" t="n">
-        <v>11.03548387096775</v>
+        <v>11.59838709677419</v>
       </c>
       <c r="H3" t="n">
-        <v>3.223387096774193</v>
+        <v>3.642741935483873</v>
       </c>
     </row>
     <row r="4">
@@ -564,22 +564,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.02741935483870966</v>
+        <v>1.203225806451613</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.429838709677419</v>
+        <v>1.265322580645161</v>
       </c>
       <c r="E4" t="n">
-        <v>-2.633870967741936</v>
+        <v>-1.523387096774194</v>
       </c>
       <c r="F4" t="n">
-        <v>9.137903225806451</v>
+        <v>11.20564516129032</v>
       </c>
       <c r="G4" t="n">
-        <v>-2.034677419354838</v>
+        <v>-1.191129032258064</v>
       </c>
       <c r="H4" t="n">
-        <v>-3.930645161290322</v>
+        <v>-2.838709677419355</v>
       </c>
     </row>
     <row r="5">
@@ -590,22 +590,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5322580645161291</v>
+        <v>0.428225806451613</v>
       </c>
       <c r="D5" t="n">
-        <v>2.053225806451612</v>
+        <v>2.819354838709677</v>
       </c>
       <c r="E5" t="n">
-        <v>4.515322580645163</v>
+        <v>4.926612903225809</v>
       </c>
       <c r="F5" t="n">
-        <v>18.28064516129032</v>
+        <v>18.78629032258064</v>
       </c>
       <c r="G5" t="n">
-        <v>12.37177419354838</v>
+        <v>13.07661290322581</v>
       </c>
       <c r="H5" t="n">
-        <v>3.791935483870968</v>
+        <v>4.187096774193548</v>
       </c>
     </row>
     <row r="6">
@@ -620,22 +620,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.3725806451612903</v>
+        <v>0.1338709677419355</v>
       </c>
       <c r="D6" t="n">
-        <v>1.008870967741936</v>
+        <v>1.532258064516129</v>
       </c>
       <c r="E6" t="n">
-        <v>4.465322580645162</v>
+        <v>4.509677419354838</v>
       </c>
       <c r="F6" t="n">
-        <v>15.07661290322581</v>
+        <v>14.94838709677419</v>
       </c>
       <c r="G6" t="n">
-        <v>13.98306451612903</v>
+        <v>13.84354838709677</v>
       </c>
       <c r="H6" t="n">
-        <v>4.741935483870967</v>
+        <v>4.733064516129032</v>
       </c>
     </row>
     <row r="7">
@@ -646,22 +646,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.1387096774193548</v>
+        <v>1.700806451612903</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.01451612903225817</v>
+        <v>3.114516129032256</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.8588709677419355</v>
+        <v>0.8137096774193551</v>
       </c>
       <c r="F7" t="n">
-        <v>13.09032258064516</v>
+        <v>15.73467741935484</v>
       </c>
       <c r="G7" t="n">
-        <v>-2.711290322580646</v>
+        <v>-0.5782258064516129</v>
       </c>
       <c r="H7" t="n">
-        <v>-3.050806451612903</v>
+        <v>-1.450806451612904</v>
       </c>
     </row>
     <row r="8">
@@ -676,22 +676,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.4103999999999999</v>
+        <v>1.3688</v>
       </c>
       <c r="D8" t="n">
-        <v>1.0504</v>
+        <v>3.395999999999999</v>
       </c>
       <c r="E8" t="n">
-        <v>2.956</v>
+        <v>4.1232</v>
       </c>
       <c r="F8" t="n">
-        <v>17.716</v>
+        <v>19.8624</v>
       </c>
       <c r="G8" t="n">
-        <v>5.544</v>
+        <v>7.4296</v>
       </c>
       <c r="H8" t="n">
-        <v>0.648</v>
+        <v>1.8144</v>
       </c>
     </row>
     <row r="9">
@@ -702,22 +702,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.2207999999999999</v>
+        <v>0.2792</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2943999999999999</v>
+        <v>1.332800000000001</v>
       </c>
       <c r="E9" t="n">
-        <v>1.372</v>
+        <v>1.617599999999999</v>
       </c>
       <c r="F9" t="n">
-        <v>9.385600000000002</v>
+        <v>10.112</v>
       </c>
       <c r="G9" t="n">
-        <v>7.556799999999999</v>
+        <v>7.529599999999998</v>
       </c>
       <c r="H9" t="n">
-        <v>1.5368</v>
+        <v>1.7832</v>
       </c>
     </row>
     <row r="10">
@@ -732,22 +732,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.02720000000000003</v>
+        <v>0.7536</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6368</v>
+        <v>2.4064</v>
       </c>
       <c r="E10" t="n">
-        <v>2.7168</v>
+        <v>3.3104</v>
       </c>
       <c r="F10" t="n">
-        <v>23.612</v>
+        <v>24.3456</v>
       </c>
       <c r="G10" t="n">
-        <v>16.828</v>
+        <v>18.228</v>
       </c>
       <c r="H10" t="n">
-        <v>2.1376</v>
+        <v>2.768800000000001</v>
       </c>
     </row>
     <row r="11">
@@ -758,22 +758,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1400000000000001</v>
+        <v>1.0912</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.1512000000000001</v>
+        <v>2.159200000000001</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.6728</v>
+        <v>0.7479999999999987</v>
       </c>
       <c r="F11" t="n">
-        <v>1.420799999999999</v>
+        <v>3.375999999999997</v>
       </c>
       <c r="G11" t="n">
-        <v>-8.1168</v>
+        <v>-7.343548387096773</v>
       </c>
       <c r="H11" t="n">
-        <v>-2.56</v>
+        <v>-1.2976</v>
       </c>
     </row>
     <row r="12">
@@ -788,22 +788,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.3712000000000001</v>
+        <v>1.0616</v>
       </c>
       <c r="D12" t="n">
-        <v>1.9008</v>
+        <v>3.4856</v>
       </c>
       <c r="E12" t="n">
-        <v>4.7736</v>
+        <v>5.825600000000001</v>
       </c>
       <c r="F12" t="n">
-        <v>22.5584</v>
+        <v>24.316</v>
       </c>
       <c r="G12" t="n">
-        <v>11.056</v>
+        <v>13.1248</v>
       </c>
       <c r="H12" t="n">
-        <v>1.9376</v>
+        <v>2.9248</v>
       </c>
     </row>
     <row r="13">
@@ -814,22 +814,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.1368</v>
+        <v>0.62</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.9431999999999999</v>
+        <v>0.7199999999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>-1.1528</v>
+        <v>-0.5568</v>
       </c>
       <c r="F13" t="n">
-        <v>4.9112</v>
+        <v>5.396</v>
       </c>
       <c r="G13" t="n">
-        <v>0.4491935483870961</v>
+        <v>0.7701612903225794</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.2616</v>
+        <v>0.3288000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>